<commit_message>
Fix: Production sync issues, Overtime logic, and Type Safety Audit improvements
</commit_message>
<xml_diff>
--- a/Reports/ESG.xlsx
+++ b/Reports/ESG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iese365-my.sharepoint.com/personal/harel_lichtenstein_iese_net/Documents/Desktop/IESE/EMBA 2026/Term 5/Executive Management Simulation - B-E1/Session 1/Report Samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iese365-my.sharepoint.com/personal/harel_lichtenstein_iese_net/Documents/Desktop/AI Tests/EXSIM models/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27ED689C-8540-44E6-9723-544D05784EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{27ED689C-8540-44E6-9723-544D05784EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFB1D527-6D46-4403-BC5E-74ABE45BCDEB}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="3570" windowWidth="21555" windowHeight="18030" xr2:uid="{292A857F-E328-46AA-96E9-908659728070}"/>
+    <workbookView xWindow="12540" yWindow="1560" windowWidth="38280" windowHeight="18030" xr2:uid="{292A857F-E328-46AA-96E9-908659728070}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -918,14 +918,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1304,673 +1304,676 @@
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="4" t="s">
+      <c r="H6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="4" t="s">
+      <c r="H7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="4" t="s">
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="4" t="s">
+      <c r="H9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="4" t="s">
+      <c r="H10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="4" t="s">
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="5" t="s">
+      <c r="H12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="4" t="s">
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="4" t="s">
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="4" t="s">
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M17" s="5" t="s">
+      <c r="H17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M19" s="6" t="s">
+      <c r="H19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1980,306 +1983,306 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="L22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="M22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M23" s="4" t="s">
+      <c r="H23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M24" s="4" t="s">
+      <c r="H24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M24" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M25" s="4" t="s">
+      <c r="B25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M25" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M26" s="4" t="s">
+      <c r="H26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M26" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M27" s="4" t="s">
+      <c r="H27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M27" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M28" s="4" t="s">
+      <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M28" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2289,147 +2292,147 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2439,147 +2442,147 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="B43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E44" s="4" t="s">
+      <c r="B44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="B45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" s="4" t="s">
+      <c r="B46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E47" s="4" t="s">
+      <c r="B47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="B48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2589,147 +2592,147 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2739,224 +2742,224 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I61" s="3" t="s">
+      <c r="I61" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J61" s="3" t="s">
+      <c r="J61" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="K61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L61" s="3" t="s">
+      <c r="L61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M61" s="3" t="s">
+      <c r="M61" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L62" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M62" s="4" t="s">
+      <c r="B62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M62" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L63" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M63" s="4" t="s">
+      <c r="B63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M63" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F64" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G64" s="4" t="s">
+      <c r="G64" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H64" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L64" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M64" s="4" t="s">
+      <c r="H64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M64" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G65" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H65" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L65" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M65" s="4" t="s">
+      <c r="H65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M65" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>